<commit_message>
Upload new data and preprocess code
</commit_message>
<xml_diff>
--- a/release/dev/ca_data/300365251.pdf.xlsx
+++ b/release/dev/ca_data/300365251.pdf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cinnamon\nlp_live_demo\bidding documents\all_bidding_ca\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaowh/Downloads/bidding_document_dataset/release/dev/ca_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DAEA3C-21DC-42CB-8460-CD3EDB0B980A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3563DEA-89D2-7A44-B7CE-786D9E69E459}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1310,11 +1310,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="G134" sqref="G134"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.6640625" customWidth="1"/>
     <col min="2" max="2" width="77.6640625" customWidth="1"/>
@@ -1323,7 +1323,7 @@
     <col min="7" max="8" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>1</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>1</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>1</v>
       </c>
@@ -1582,7 +1582,7 @@
       </c>
       <c r="G12" s="40"/>
     </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>1</v>
       </c>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="G13" s="40"/>
     </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>1</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>1</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>1</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>1</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>1</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>1</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>1</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>1</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>1</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>1</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>1</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>1</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>1</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>1</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>1</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>1</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>1</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>1</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>2</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>2</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>2</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>2</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>2</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>2</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>2</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>2</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>2</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>2</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>2</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>2</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>2</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>2</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>2</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>2</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>2</v>
       </c>
@@ -2413,7 +2413,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>2</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>2</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>2</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>2</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>2</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>2</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>2</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>2</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>2</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>2</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>2</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>2</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>2</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>2</v>
       </c>
@@ -2693,7 +2693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>2</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>2</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>2</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>2</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>3</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>3</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>3</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>3</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>3</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>3</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>3</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>3</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>3</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>3</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>3</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>3</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>3</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>3</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>3</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>3</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4">
         <v>3</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4">
         <v>3</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4">
         <v>3</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4">
         <v>3</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>3</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>3</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4">
         <v>3</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4">
         <v>3</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4">
         <v>3</v>
       </c>
@@ -3334,10 +3334,10 @@
         <v>200</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>3</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4">
         <v>3</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4">
         <v>3</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4">
         <v>3</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4">
         <v>3</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4">
         <v>3</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4">
         <v>3</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>3</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4">
         <v>3</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4">
         <v>3</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4">
         <v>4</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4">
         <v>4</v>
       </c>
@@ -3601,7 +3601,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4">
         <v>4</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4">
         <v>4</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>4</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
         <v>4</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>4</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>4</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
         <v>4</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>4</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
         <v>4</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
         <v>4</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>4</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
         <v>4</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>4</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
         <v>4</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
         <v>4</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>4</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>4</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>4</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
         <v>4</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
         <v>4</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
         <v>4</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
         <v>4</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
         <v>4</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>4</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
         <v>4</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
         <v>4</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>4</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4">
         <v>4</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4">
         <v>4</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>4</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>4</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4">
         <v>5</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4">
         <v>5</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
         <v>5</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
         <v>5</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
         <v>5</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
         <v>5</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
         <v>5</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
         <v>5</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4">
         <v>5</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4">
         <v>5</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4">
         <v>5</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="4">
         <v>5</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="4">
         <v>5</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4">
         <v>5</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="4">
         <v>5</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="4">
         <v>5</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="4">
         <v>5</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="4">
         <v>5</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>5</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="4">
         <v>5</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="4">
         <v>5</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="4">
         <v>5</v>
       </c>
@@ -4661,7 +4661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="4">
         <v>5</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="4">
         <v>5</v>
       </c>
@@ -4701,7 +4701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="4">
         <v>5</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="4">
         <v>5</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="4">
         <v>5</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="4">
         <v>5</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="4">
         <v>5</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="4">
         <v>5</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="4">
         <v>5</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="4">
         <v>5</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="4">
         <v>5</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="4">
         <v>5</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="4">
         <v>5</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="4">
         <v>6</v>
       </c>
@@ -4941,7 +4941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="4">
         <v>6</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="4">
         <v>6</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="4">
         <v>6</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="4">
         <v>6</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="4">
         <v>6</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="4">
         <v>6</v>
       </c>

</xml_diff>